<commit_message>
Just checking in some trivial updates.
</commit_message>
<xml_diff>
--- a/Notebooks/covid-19-caution/countries.xlsx
+++ b/Notebooks/covid-19-caution/countries.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/projects/Covid-19/covid-recovery/Notebooks/covid-19-caution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2D0491-9AEA-D540-BFE9-29B4D1E70E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74797582-464D-994C-9372-5B13CCED1B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6740" yWindow="3420" windowWidth="27240" windowHeight="16440" xr2:uid="{7C607F7F-AC8B-EF46-954B-802A2A5CFBF3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="188">
   <si>
     <t>'Afghanistan'</t>
   </si>
@@ -989,12 +990,261 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE12EC34-2937-7F46-A5EE-C487593B61A5}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A67">
+    <sortCondition ref="A1:A67"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6310402A-76CF-8649-838D-434A2FBCBD3C}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1285,7 +1535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F334D0A7-238A-454D-92CF-A1253BA5023C}">
   <dimension ref="A1:CC81"/>
   <sheetViews>
@@ -2025,7 +2275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD17805-4207-584A-84EF-2D5246F020A5}">
   <dimension ref="A1:F32"/>
   <sheetViews>
@@ -2676,7 +2926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6876CE91-6DDF-A34D-B691-48BB7C8B0FD2}">
   <dimension ref="A1:GE187"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fixed final date of data set to Oct 9th in data.py. Can be changed there. Debugged same length offset datasets. Changes to manuscript accepted with slight modifications in version 8.
</commit_message>
<xml_diff>
--- a/Notebooks/covid-19-caution/countries.xlsx
+++ b/Notebooks/covid-19-caution/countries.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/projects/Covid-19/covid-recovery/Notebooks/covid-19-caution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74797582-464D-994C-9372-5B13CCED1B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD66A42C-78CE-344B-B6F0-BE557F1A094C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6740" yWindow="3420" windowWidth="27240" windowHeight="16440" xr2:uid="{7C607F7F-AC8B-EF46-954B-802A2A5CFBF3}"/>
+    <workbookView xWindow="6420" yWindow="2000" windowWidth="27240" windowHeight="16440" xr2:uid="{7C607F7F-AC8B-EF46-954B-802A2A5CFBF3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet5" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="lbcountries" sheetId="5" r:id="rId1"/>
+    <sheet name="bcountries" sheetId="4" r:id="rId2"/>
+    <sheet name="bcountries raw" sheetId="3" r:id="rId3"/>
+    <sheet name="ccountries" sheetId="2" r:id="rId4"/>
+    <sheet name="ccountries raw" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="188">
   <si>
     <t>'Afghanistan'</t>
   </si>
@@ -630,19 +630,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12.5"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="17"/>
@@ -671,12 +665,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE12EC34-2937-7F46-A5EE-C487593B61A5}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F12"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1021,10 +1012,10 @@
         <v>87</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1041,10 +1032,10 @@
         <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1061,10 +1052,10 @@
         <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1078,13 +1069,13 @@
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1098,13 +1089,13 @@
         <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1118,13 +1109,13 @@
         <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1138,13 +1129,13 @@
         <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F7" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1158,10 +1149,13 @@
         <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>132</v>
+      </c>
+      <c r="F8" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1175,10 +1169,10 @@
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1192,10 +1186,10 @@
         <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1209,10 +1203,10 @@
         <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1226,11 +1220,47 @@
         <v>86</v>
       </c>
       <c r="D12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
-        <v>150</v>
-      </c>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="23" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="23" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" ht="23" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" ht="23" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" ht="23" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" ht="23" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" ht="23" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" ht="23" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" ht="23" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" ht="23" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" ht="23" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" ht="23" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A67">
@@ -1242,294 +1272,691 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6310402A-76CF-8649-838D-434A2FBCBD3C}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="C1:H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>187</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" t="s">
         <v>181</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" t="s">
-        <v>174</v>
-      </c>
       <c r="F1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>70</v>
       </c>
-      <c r="D2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" t="s">
-        <v>123</v>
-      </c>
       <c r="F2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>71</v>
       </c>
-      <c r="D3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" t="s">
-        <v>125</v>
-      </c>
       <c r="F3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+      <c r="G3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>73</v>
       </c>
-      <c r="D4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" t="s">
-        <v>126</v>
-      </c>
       <c r="F4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="G4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>180</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>75</v>
       </c>
-      <c r="D5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" t="s">
-        <v>127</v>
-      </c>
       <c r="F5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="G5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>76</v>
       </c>
-      <c r="D6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" t="s">
-        <v>128</v>
-      </c>
       <c r="F6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="G6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>77</v>
       </c>
-      <c r="D7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" t="s">
-        <v>129</v>
-      </c>
       <c r="F7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="G7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
         <v>47</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>78</v>
       </c>
-      <c r="D8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" t="s">
-        <v>130</v>
-      </c>
       <c r="F8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
         <v>48</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>79</v>
       </c>
-      <c r="D9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" t="s">
-        <v>131</v>
-      </c>
       <c r="F9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="G9" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
         <v>49</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>80</v>
       </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>132</v>
-      </c>
       <c r="F10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="G10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" t="s">
-        <v>113</v>
-      </c>
       <c r="E11" t="s">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="F11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="G11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
         <v>58</v>
       </c>
-      <c r="C12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
-      </c>
       <c r="E12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
         <v>60</v>
       </c>
-      <c r="C13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" t="s">
-        <v>121</v>
-      </c>
       <c r="E13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+      <c r="F13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
         <v>62</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>88</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>122</v>
       </c>
-      <c r="E14" t="s">
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>148</v>
       </c>
     </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A82">
-    <sortCondition ref="A1:A82"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A84">
+    <sortCondition ref="A1:A84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1537,16 +1964,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F334D0A7-238A-454D-92CF-A1253BA5023C}">
-  <dimension ref="A1:CC81"/>
+  <dimension ref="A1:CE83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A81"/>
+      <selection sqref="A1:A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:81" ht="23" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1661,220 +2088,226 @@
         <v>80</v>
       </c>
       <c r="AM1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN1" t="s">
         <v>83</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>86</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>87</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>88</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>91</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>94</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU1" t="s">
         <v>97</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>104</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>106</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>107</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>110</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AZ1" t="s">
         <v>111</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
         <v>113</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BB1" t="s">
         <v>119</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BC1" t="s">
         <v>120</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>121</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>122</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
         <v>123</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BG1" t="s">
         <v>125</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BH1" t="s">
         <v>126</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BI1" t="s">
         <v>127</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BJ1" t="s">
         <v>128</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BK1" t="s">
         <v>129</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BL1" t="s">
         <v>130</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BM1" t="s">
         <v>131</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BN1" t="s">
         <v>132</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BO1" t="s">
         <v>139</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BP1" t="s">
         <v>141</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BQ1" t="s">
         <v>146</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BR1" t="s">
         <v>148</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BS1" t="s">
         <v>150</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BT1" t="s">
         <v>153</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BU1" t="s">
         <v>154</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BV1" t="s">
         <v>155</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BW1" t="s">
         <v>164</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BX1" t="s">
         <v>165</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BY1" t="s">
         <v>166</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BZ1" t="s">
         <v>168</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CA1" t="s">
         <v>169</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CB1" t="s">
         <v>174</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CC1" t="s">
         <v>177</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CD1" t="s">
         <v>180</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CE1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A2" t="str" cm="1">
         <f t="array" aca="1" ref="A2" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Albania'</v>
       </c>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A3" t="str" cm="1">
         <f t="array" aca="1" ref="A3" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Argentina'</v>
       </c>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A4" t="str" cm="1">
         <f t="array" aca="1" ref="A4" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Armenia'</v>
       </c>
     </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A5" t="str" cm="1">
         <f t="array" aca="1" ref="A5" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Austria'</v>
       </c>
     </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A6" t="str" cm="1">
         <f t="array" aca="1" ref="A6" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Azerbaijan'</v>
       </c>
     </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A7" t="str" cm="1">
         <f t="array" aca="1" ref="A7" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Bahrain'</v>
       </c>
     </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A8" t="str" cm="1">
         <f t="array" aca="1" ref="A8" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Belarus'</v>
       </c>
     </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A9" t="str" cm="1">
         <f t="array" aca="1" ref="A9" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Belgium'</v>
       </c>
     </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A10" t="str" cm="1">
         <f t="array" aca="1" ref="A10" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Bolivia'</v>
       </c>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A11" t="str" cm="1">
         <f t="array" aca="1" ref="A11" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Bosnia and Herzegovina'</v>
       </c>
     </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A12" t="str" cm="1">
         <f t="array" aca="1" ref="A12" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Brazil'</v>
       </c>
     </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A13" t="str" cm="1">
         <f t="array" aca="1" ref="A13" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Bulgaria'</v>
       </c>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A14" t="str" cm="1">
         <f t="array" aca="1" ref="A14" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Myanmar'</v>
       </c>
     </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A15" t="str" cm="1">
         <f t="array" aca="1" ref="A15" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Chile'</v>
       </c>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A16" t="str" cm="1">
         <f t="array" aca="1" ref="A16" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Colombia'</v>
@@ -2015,258 +2448,270 @@
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="str" cm="1">
         <f t="array" aca="1" ref="A39" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Kazakhstan'</v>
+        <v xml:space="preserve"> 'Jordan'</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="str" cm="1">
         <f t="array" aca="1" ref="A40" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Kosovo'</v>
+        <v xml:space="preserve"> 'Kazakhstan'</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="str" cm="1">
         <f t="array" aca="1" ref="A41" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Kuwait'</v>
+        <v xml:space="preserve"> 'Kosovo'</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="str" cm="1">
         <f t="array" aca="1" ref="A42" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Kyrgyzstan'</v>
+        <v xml:space="preserve"> 'Kuwait'</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="str" cm="1">
         <f t="array" aca="1" ref="A43" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Lebanon'</v>
+        <v xml:space="preserve"> 'Kyrgyzstan'</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="str" cm="1">
         <f t="array" aca="1" ref="A44" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Libya'</v>
+        <v xml:space="preserve"> 'Lebanon'</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="str" cm="1">
         <f t="array" aca="1" ref="A45" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Luxembourg'</v>
+        <v xml:space="preserve"> 'Libya'</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="str" cm="1">
         <f t="array" aca="1" ref="A46" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Mauritania'</v>
+        <v xml:space="preserve"> 'Lithuania'</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="str" cm="1">
         <f t="array" aca="1" ref="A47" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Mexico'</v>
+        <v xml:space="preserve"> 'Luxembourg'</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="str" cm="1">
         <f t="array" aca="1" ref="A48" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Moldova'</v>
+        <v xml:space="preserve"> 'Mauritania'</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="str" cm="1">
         <f t="array" aca="1" ref="A49" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Montenegro'</v>
+        <v xml:space="preserve"> 'Mexico'</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="str" cm="1">
         <f t="array" aca="1" ref="A50" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Morocco'</v>
+        <v xml:space="preserve"> 'Moldova'</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="str" cm="1">
         <f t="array" aca="1" ref="A51" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Namibia'</v>
+        <v xml:space="preserve"> 'Montenegro'</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="str" cm="1">
         <f t="array" aca="1" ref="A52" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Macedonia'</v>
+        <v xml:space="preserve"> 'Morocco'</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="str" cm="1">
         <f t="array" aca="1" ref="A53" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Norway'</v>
+        <v xml:space="preserve"> 'Namibia'</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="str" cm="1">
         <f t="array" aca="1" ref="A54" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Oman'</v>
+        <v xml:space="preserve"> 'Macedonia'</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="str" cm="1">
         <f t="array" aca="1" ref="A55" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Pakistan'</v>
+        <v xml:space="preserve"> 'Norway'</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="str" cm="1">
         <f t="array" aca="1" ref="A56" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Panama'</v>
+        <v xml:space="preserve"> 'Oman'</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="str" cm="1">
         <f t="array" aca="1" ref="A57" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Paraguay'</v>
+        <v xml:space="preserve"> 'Pakistan'</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="str" cm="1">
         <f t="array" aca="1" ref="A58" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Peru'</v>
+        <v xml:space="preserve"> 'Panama'</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="str" cm="1">
         <f t="array" aca="1" ref="A59" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Philippines'</v>
+        <v xml:space="preserve"> 'Paraguay'</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="str" cm="1">
         <f t="array" aca="1" ref="A60" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Poland'</v>
+        <v xml:space="preserve"> 'Peru'</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="str" cm="1">
         <f t="array" aca="1" ref="A61" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Portugal'</v>
+        <v xml:space="preserve"> 'Philippines'</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="str" cm="1">
         <f t="array" aca="1" ref="A62" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Qatar'</v>
+        <v xml:space="preserve"> 'Poland'</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="str" cm="1">
         <f t="array" aca="1" ref="A63" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Romania'</v>
+        <v xml:space="preserve"> 'Portugal'</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="str" cm="1">
         <f t="array" aca="1" ref="A64" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Russia'</v>
+        <v xml:space="preserve"> 'Qatar'</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="str" cm="1">
         <f t="array" aca="1" ref="A65" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Saudi Arabia'</v>
+        <v xml:space="preserve"> 'Romania'</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="str" cm="1">
         <f t="array" aca="1" ref="A66" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Serbia'</v>
+        <v xml:space="preserve"> 'Russia'</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="str" cm="1">
         <f t="array" aca="1" ref="A67" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Slovenia'</v>
+        <v xml:space="preserve"> 'Saudi Arabia'</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="str" cm="1">
         <f t="array" aca="1" ref="A68" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'South Africa'</v>
+        <v xml:space="preserve"> 'Serbia'</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="str" cm="1">
         <f t="array" aca="1" ref="A69" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Spain'</v>
+        <v xml:space="preserve"> 'Slovenia'</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="str" cm="1">
         <f t="array" aca="1" ref="A70" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Suriname'</v>
+        <v xml:space="preserve"> 'South Africa'</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="str" cm="1">
         <f t="array" aca="1" ref="A71" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Sweden'</v>
+        <v xml:space="preserve"> 'Spain'</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="str" cm="1">
         <f t="array" aca="1" ref="A72" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Switzerland'</v>
+        <v xml:space="preserve"> 'Suriname'</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="str" cm="1">
         <f t="array" aca="1" ref="A73" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Tunisia'</v>
+        <v xml:space="preserve"> 'Sweden'</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="str" cm="1">
         <f t="array" aca="1" ref="A74" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Turkey'</v>
+        <v xml:space="preserve"> 'Switzerland'</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="str" cm="1">
         <f t="array" aca="1" ref="A75" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'United States'</v>
+        <v xml:space="preserve"> 'Tunisia'</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="str" cm="1">
         <f t="array" aca="1" ref="A76" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Ukraine'</v>
+        <v xml:space="preserve"> 'Turkey'</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="str" cm="1">
         <f t="array" aca="1" ref="A77" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'United Arab Emirates'</v>
+        <v xml:space="preserve"> 'United States'</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="str" cm="1">
         <f t="array" aca="1" ref="A78" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Palestine'</v>
+        <v xml:space="preserve"> 'Ukraine'</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="str" cm="1">
         <f t="array" aca="1" ref="A79" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Zambia'</v>
+        <v xml:space="preserve"> 'United Arab Emirates'</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="str" cm="1">
         <f t="array" aca="1" ref="A80" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
-        <v xml:space="preserve"> 'Australia'</v>
+        <v xml:space="preserve"> 'Palestine'</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="str" cm="1">
         <f t="array" aca="1" ref="A81" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
+        <v xml:space="preserve"> 'Zambia'</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="str" cm="1">
+        <f t="array" aca="1" ref="A82" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
+        <v xml:space="preserve"> 'Australia'</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="str" cm="1">
+        <f t="array" aca="1" ref="A83" ca="1">INDIRECT(ADDRESS(1,ROW()))</f>
         <v xml:space="preserve"> 'Canada'</v>
       </c>
     </row>
@@ -2931,7 +3376,7 @@
   <dimension ref="A1:GE187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2939,9 +3384,9 @@
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:187" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:187" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>187</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>

</xml_diff>